<commit_message>
case study meta data
</commit_message>
<xml_diff>
--- a/case_study_analysis/cf_scripts/data/case_study_meta_data.xlsx
+++ b/case_study_analysis/cf_scripts/data/case_study_meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/cc_resilience/climate-resilient-fisheries/case_study_analysis/cf_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA476E26-B44E-AA4B-9941-45281261D4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360BE065-2629-7A48-99BA-463D22FFFFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21100" yWindow="2340" windowWidth="28040" windowHeight="17440" xr2:uid="{64AC2A7C-3AC6-264D-A117-FA5C5DCDB163}"/>
   </bookViews>
@@ -626,7 +626,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data cleaning and fig 1
</commit_message>
<xml_diff>
--- a/case_study_analysis/cf_scripts/data/case_study_meta_data.xlsx
+++ b/case_study_analysis/cf_scripts/data/case_study_meta_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/cc_resilience/climate-resilient-fisheries/case_study_analysis/cf_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360BE065-2629-7A48-99BA-463D22FFFFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD04DFBE-428A-5249-A0F9-F7A05659FBE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21100" yWindow="2340" windowWidth="28040" windowHeight="17440" xr2:uid="{64AC2A7C-3AC6-264D-A117-FA5C5DCDB163}"/>
   </bookViews>
@@ -18,20 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$18</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -232,9 +222,6 @@
     <t>Madagascar nearshore</t>
   </si>
   <si>
-    <t>Alaska Bering Sea groundfish</t>
-  </si>
-  <si>
     <t>Maine American lobster</t>
   </si>
   <si>
@@ -251,6 +238,9 @@
   </si>
   <si>
     <t>Moorea reef fish</t>
+  </si>
+  <si>
+    <t>US Bering Sea groundfish</t>
   </si>
 </sst>
 </file>
@@ -626,7 +616,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,7 +929,7 @@
         <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>53</v>
@@ -975,7 +965,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>55</v>
@@ -1011,7 +1001,7 @@
         <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>53</v>
@@ -1119,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>54</v>
@@ -1191,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>54</v>
@@ -1227,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>53</v>
@@ -1263,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>53</v>
@@ -1329,7 +1319,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K18" xr:uid="{AEE2DA7E-BB06-9C4E-BB11-C7D5A6AED76B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K18">
+    <sortState ref="A2:K18">
       <sortCondition ref="A1:A18"/>
     </sortState>
   </autoFilter>

</xml_diff>